<commit_message>
Adding Presentation Layer First Commit
</commit_message>
<xml_diff>
--- a/Banking Mini Project/data/BankingData.xlsx
+++ b/Banking Mini Project/data/BankingData.xlsx
@@ -8,18 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/renga/Documents/SpringBoard Data Engineering Course/bankingEnv/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDAA4A16-6850-C446-8288-A3005C504A43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A80B6BE9-A672-1C4F-9FC6-A48330E136F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5220" yWindow="1320" windowWidth="28040" windowHeight="16420" activeTab="3" xr2:uid="{53CE078C-3FFB-5942-8CD9-E853A9DE31EF}"/>
+    <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="16420" xr2:uid="{53CE078C-3FFB-5942-8CD9-E853A9DE31EF}"/>
   </bookViews>
   <sheets>
     <sheet name="Employees" sheetId="1" r:id="rId1"/>
     <sheet name="Customers" sheetId="2" r:id="rId2"/>
     <sheet name="AccountServices" sheetId="3" r:id="rId3"/>
     <sheet name="LoanServices" sheetId="4" r:id="rId4"/>
-    <sheet name="CreditCardServices" sheetId="5" r:id="rId5"/>
-    <sheet name="CustomerAccountSummary" sheetId="8" r:id="rId6"/>
-    <sheet name="CustomerAccountDetail" sheetId="9" r:id="rId7"/>
+    <sheet name="CustomerAccountSummary" sheetId="8" r:id="rId5"/>
+    <sheet name="CustomerAccountDetail" sheetId="9" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -41,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="141">
   <si>
     <t>Id</t>
   </si>
@@ -115,12 +114,6 @@
     <t>MaximumCreditScore</t>
   </si>
   <si>
-    <t>MaximumCreditLimit</t>
-  </si>
-  <si>
-    <t>OneYearSecurityDeposit</t>
-  </si>
-  <si>
     <t>E000000001</t>
   </si>
   <si>
@@ -370,30 +363,6 @@
     <t>36</t>
   </si>
   <si>
-    <t>CS0001</t>
-  </si>
-  <si>
-    <t>Visa</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>CS0002</t>
-  </si>
-  <si>
-    <t>CS0003</t>
-  </si>
-  <si>
-    <t>CS0004</t>
-  </si>
-  <si>
-    <t>MasterCard</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
     <t>AddressLine2</t>
   </si>
   <si>
@@ -442,9 +411,6 @@
     <t>LoanServiceId</t>
   </si>
   <si>
-    <t>CreditCardServiceId</t>
-  </si>
-  <si>
     <t>AccountDetailId</t>
   </si>
   <si>
@@ -463,16 +429,7 @@
     <t>LoanCostPercentage</t>
   </si>
   <si>
-    <t>MinimumCreditScore</t>
-  </si>
-  <si>
     <t>PeriodInMonths</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>YearlyFees</t>
   </si>
   <si>
     <t>No</t>
@@ -898,7 +855,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8CA3977-E658-B346-90DA-19FCDF11AF9C}">
   <dimension ref="A1:O6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
@@ -934,7 +891,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
@@ -969,222 +926,222 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="F2" t="s">
         <v>32</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G2" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="F2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>35</v>
       </c>
       <c r="H2">
         <v>30339</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="N2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="O2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="F3" t="s">
         <v>40</v>
       </c>
-      <c r="D3" t="s">
-        <v>41</v>
-      </c>
-      <c r="F3" t="s">
-        <v>42</v>
-      </c>
       <c r="G3" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H3">
         <v>30041</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
       <c r="N3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="O3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H4">
         <v>30320</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="N4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="O4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" t="s">
         <v>48</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D5" t="s">
-        <v>50</v>
-      </c>
       <c r="F5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H5">
         <v>30339</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="N5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="O5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" t="s">
         <v>51</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="F6" t="s">
         <v>52</v>
       </c>
-      <c r="D6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F6" t="s">
-        <v>54</v>
-      </c>
       <c r="G6" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H6">
         <v>30024</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
       <c r="N6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="O6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1218,7 +1175,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1230,7 +1187,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
@@ -1248,7 +1205,7 @@
         <v>14</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>15</v>
@@ -1262,198 +1219,198 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="F2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>35</v>
       </c>
       <c r="H2">
         <v>30339</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H3">
         <v>30041</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H4">
         <v>30320</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="L4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H5">
         <v>30339</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H6">
         <v>30024</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J6" t="s">
+        <v>69</v>
+      </c>
+      <c r="K6" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="K6" s="2" t="s">
-        <v>73</v>
-      </c>
       <c r="L6" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1489,10 +1446,10 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>23</v>
@@ -1501,13 +1458,13 @@
         <v>17</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>22</v>
@@ -1516,7 +1473,7 @@
         <v>18</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>11</v>
@@ -1527,234 +1484,234 @@
     </row>
     <row r="2" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>19</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
       <c r="I2">
         <v>10000</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="O2" s="5"/>
     </row>
     <row r="3" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>19</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
       <c r="I3">
         <v>10000</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="O3" s="6"/>
     </row>
     <row r="4" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>78</v>
-      </c>
       <c r="E4" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>150</v>
+        <v>136</v>
       </c>
       <c r="I4">
         <v>15000</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="E5" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>78</v>
-      </c>
       <c r="F5" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="H5" s="8" t="s">
         <v>137</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>151</v>
       </c>
       <c r="I5">
         <v>25000</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="O5" s="5"/>
     </row>
     <row r="6" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B6" t="s">
-        <v>84</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>85</v>
-      </c>
       <c r="D6" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>152</v>
+        <v>138</v>
       </c>
       <c r="I6">
         <v>10000</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="O6" s="5"/>
     </row>
     <row r="7" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
       <c r="I7">
         <v>10000</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="O7" s="5"/>
     </row>
@@ -1767,7 +1724,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F8A9F79-3B49-5C40-A490-3D6F93CA8129}">
   <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
@@ -1786,10 +1743,10 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>20</v>
@@ -1801,13 +1758,13 @@
         <v>22</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>148</v>
+        <v>134</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>11</v>
@@ -1818,22 +1775,22 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C2">
         <v>1000</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>89</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>91</v>
       </c>
       <c r="G2" s="9">
         <v>2</v>
@@ -1842,30 +1799,30 @@
         <v>20</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C3">
         <v>10000</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G3" s="9">
         <v>2.5</v>
@@ -1874,32 +1831,32 @@
         <v>60</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="K3" s="7"/>
       <c r="L3" s="7"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C4">
         <v>75000</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>154</v>
+        <v>140</v>
       </c>
       <c r="G4" s="9">
         <v>2</v>
@@ -1908,32 +1865,32 @@
         <v>200</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="K4" s="7"/>
       <c r="L4" s="7"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C5">
         <v>150000</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>154</v>
+        <v>140</v>
       </c>
       <c r="G5" s="9">
         <v>2.5</v>
@@ -1942,32 +1899,32 @@
         <v>300</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="K5" s="7"/>
       <c r="L5" s="7"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B6" t="s">
         <v>100</v>
-      </c>
-      <c r="B6" t="s">
-        <v>102</v>
       </c>
       <c r="C6">
         <v>1000</v>
       </c>
       <c r="D6" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>106</v>
       </c>
       <c r="G6" s="9">
         <v>2</v>
@@ -1976,30 +1933,30 @@
         <v>20</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>99</v>
+      </c>
+      <c r="B7" t="s">
         <v>101</v>
-      </c>
-      <c r="B7" t="s">
-        <v>103</v>
       </c>
       <c r="C7">
         <v>10000</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G7" s="9">
         <v>2.5</v>
@@ -2008,10 +1965,10 @@
         <v>100</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -2020,192 +1977,6 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57974CD4-C9D0-FD46-B924-3F91A35F3DEC}">
-  <dimension ref="A1:J5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="11.1640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>109</v>
-      </c>
-      <c r="B2" t="s">
-        <v>110</v>
-      </c>
-      <c r="C2">
-        <v>500</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="G2" s="9">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>100</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>112</v>
-      </c>
-      <c r="B3" t="s">
-        <v>110</v>
-      </c>
-      <c r="C3">
-        <v>15000</v>
-      </c>
-      <c r="D3">
-        <v>400</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="G3" s="9">
-        <v>15</v>
-      </c>
-      <c r="H3">
-        <v>1000</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>113</v>
-      </c>
-      <c r="B4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C4">
-        <v>30000</v>
-      </c>
-      <c r="D4">
-        <v>600</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="G4" s="9">
-        <v>30</v>
-      </c>
-      <c r="H4">
-        <v>5000</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>114</v>
-      </c>
-      <c r="B5" t="s">
-        <v>115</v>
-      </c>
-      <c r="C5">
-        <v>45000</v>
-      </c>
-      <c r="D5">
-        <v>700</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="G5" s="9">
-        <v>60</v>
-      </c>
-      <c r="H5">
-        <v>10000</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58EBC3DB-7AFA-C548-9172-806268290870}">
   <dimension ref="A1:H6"/>
   <sheetViews>
@@ -2227,22 +1998,22 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>11</v>
@@ -2253,16 +2024,16 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="C2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E2">
         <v>500</v>
@@ -2271,24 +2042,24 @@
         <v>10000</v>
       </c>
       <c r="G2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="H2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="C3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E3">
         <v>431</v>
@@ -2297,24 +2068,24 @@
         <v>5000</v>
       </c>
       <c r="G3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="H3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B4" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="C4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E4">
         <v>720</v>
@@ -2323,24 +2094,24 @@
         <v>25000</v>
       </c>
       <c r="G4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="H4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B5" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="C5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E5">
         <v>655</v>
@@ -2349,24 +2120,24 @@
         <v>30000</v>
       </c>
       <c r="G5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="H5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B6" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="C6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E6">
         <v>760</v>
@@ -2375,10 +2146,10 @@
         <v>50000</v>
       </c>
       <c r="G6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="H6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -2386,7 +2157,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD3FC9F7-F25E-7E43-A058-F8C408391786}">
   <dimension ref="A1:F11"/>
   <sheetViews>
@@ -2405,16 +2176,16 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>130</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>11</v>
@@ -2428,7 +2199,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -2437,10 +2208,10 @@
         <v>10000</v>
       </c>
       <c r="E2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -2448,7 +2219,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -2457,10 +2228,10 @@
         <v>5000</v>
       </c>
       <c r="E3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -2468,7 +2239,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -2477,10 +2248,10 @@
         <v>25000</v>
       </c>
       <c r="E4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -2488,7 +2259,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -2497,10 +2268,10 @@
         <v>30000</v>
       </c>
       <c r="E5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -2508,7 +2279,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -2517,10 +2288,10 @@
         <v>50000</v>
       </c>
       <c r="E6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -2528,7 +2299,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="C7" s="10">
         <v>200</v>
@@ -2537,10 +2308,10 @@
         <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -2548,7 +2319,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="C8" s="10">
         <v>0</v>
@@ -2557,10 +2328,10 @@
         <v>400</v>
       </c>
       <c r="E8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -2568,7 +2339,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="C9" s="10">
         <v>1000</v>
@@ -2577,10 +2348,10 @@
         <v>0</v>
       </c>
       <c r="E9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -2588,7 +2359,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="C10" s="10">
         <v>0</v>
@@ -2597,10 +2368,10 @@
         <v>2000</v>
       </c>
       <c r="E10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -2608,7 +2379,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="C11" s="10">
         <v>5000</v>
@@ -2617,10 +2388,10 @@
         <v>0</v>
       </c>
       <c r="E11" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F11" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>